<commit_message>
Subindo CSS e imagens faltantes
</commit_message>
<xml_diff>
--- a/dist/relatorio_automatico.xlsx
+++ b/dist/relatorio_automatico.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1499,6 +1499,206 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>zinter</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>meyerrfd44@gmail.com</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>66666wdafd</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>srluiz</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>luiz224@gmail.com</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>luiz3747343</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Pedro Alves cabral</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>cabral@gmail</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>cabral</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maria </t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Ju@pet</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>1212</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>erere</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>mekdafeafeaanics153@gmail.com</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>erfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JSONvc</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>mferreiradejesus11@gmail.com</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>mbnv bcxvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Gustavo</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>gustavo.vannucchi.ungari@gmail.com</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Narcelo2026=</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Sroliver</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>sroliver555@gmail.com</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>sroliver</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>tkinterr</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>102030@gmail.com</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>102030</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>zcrustess</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>mferredsdaejesus11@gmail.com</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>mnbv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>